<commit_message>
KFold now working with script
</commit_message>
<xml_diff>
--- a/Output/Training_Overview.xlsx
+++ b/Output/Training_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS479_Final_Project\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FB0D0E-4E81-48A0-AE65-CE4E25804135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7632CBCE-5403-4B4E-B372-CA09018BDED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Unprocessed_NaivePartition</t>
   </si>
@@ -39,13 +39,19 @@
     <t>Avg Recall</t>
   </si>
   <si>
-    <t>Cropped_Compensated_NaivePartition</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
     <t>Cropped_NaivePartition</t>
+  </si>
+  <si>
+    <t>Cropped_Compensated_NaivePartition_ Biased</t>
+  </si>
+  <si>
+    <t>Cropped_Compensated_NaivePartition_ Unbiased</t>
+  </si>
+  <si>
+    <t>Cropped_Compensated_5FoldPartition</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +395,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -408,7 +414,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.47299999999999998</v>
@@ -425,7 +431,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.87239999999999995</v>
@@ -438,6 +444,40 @@
       </c>
       <c r="E4">
         <v>0.83250000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.23449999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.2722</v>
+      </c>
+      <c r="D5">
+        <v>0.33379999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.38540000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.35389999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.36</v>
+      </c>
+      <c r="D6">
+        <v>0.435</v>
+      </c>
+      <c r="E6">
+        <v>0.71879999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New networks and sampling code
</commit_message>
<xml_diff>
--- a/Output/Training_Overview.xlsx
+++ b/Output/Training_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS479_Final_Project\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E31C8B-B56A-4064-BB65-C718AA68D87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28F7604-A43F-4BF9-B907-693E6A9749D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43170" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>Cropped_Compensated_NaivePartition_ Unbiased</t>
   </si>
   <si>
-    <t>Cropped_Compensated_Normalized_5FoldPartition</t>
-  </si>
-  <si>
     <t>Cropped_Compensated_1FoldPartition</t>
   </si>
   <si>
     <t>Cropped_Compensated_Normalized_1FoldPartition</t>
+  </si>
+  <si>
+    <t>Cropped_Compensated_Normalized_5FoldPartition_Test1</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.35389999999999999</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.41789999999999999</v>
@@ -505,7 +505,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.38340000000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.4607</v>
+      </c>
+      <c r="D8">
+        <v>0.52649999999999997</v>
+      </c>
+      <c r="E8">
+        <v>0.6532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>